<commit_message>
Included Jira IDs for each test case data.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval-CancelAndClose.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval-CancelAndClose.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS_Sprint5\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="Transmittals_Close_Cancel" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Transmittals_Close_Cancel!$A$1:$Q$5</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>To</t>
   </si>
@@ -100,6 +103,21 @@
   </si>
   <si>
     <t>Issued for Approval</t>
+  </si>
+  <si>
+    <t>RefID</t>
+  </si>
+  <si>
+    <t>LATFLD-24</t>
+  </si>
+  <si>
+    <t>LATFLD-23</t>
+  </si>
+  <si>
+    <t>LATFLD-17</t>
+  </si>
+  <si>
+    <t>LATFLD-12</t>
   </si>
 </sst>
 </file>
@@ -500,186 +518,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="9" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="13" width="25.85546875" customWidth="1"/>
-    <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1"/>
+    <col min="14" max="14" width="25.85546875" customWidth="1"/>
+    <col min="15" max="15" width="19" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>5</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>5</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>5</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>26</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>5</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated references of message, included overdue refID
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval-CancelAndClose.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval-CancelAndClose.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_S5_NR\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS_Sprint5\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Transmittals_Close_Cancel!$A$1:$R$5</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -674,7 +674,7 @@
         <v>26</v>
       </c>
       <c r="N3" t="str">
-        <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O2)</f>
+        <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O3)</f>
         <v>2 of 4 Message for New transmittal</v>
       </c>
       <c r="O3" t="s">
@@ -707,7 +707,7 @@
         <v>26</v>
       </c>
       <c r="N4" t="str">
-        <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O2)</f>
+        <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O4)</f>
         <v>3 of 4 Message for New transmittal</v>
       </c>
       <c r="O4" t="s">
@@ -740,7 +740,7 @@
         <v>26</v>
       </c>
       <c r="N5" t="str">
-        <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O2)</f>
+        <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O5)</f>
         <v>4 of 4 Message for New transmittal</v>
       </c>
       <c r="O5" t="s">

</xml_diff>

<commit_message>
Created Generic_Data and updated user and doc data references.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval-CancelAndClose.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval-CancelAndClose.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS_Sprint5\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Transmittals_Close_Cancel" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Transmittals_Close_Cancel!$A$1:$R$5</definedName>
   </definedNames>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>To</t>
   </si>
@@ -81,9 +84,6 @@
     <t>ReviewDocument</t>
   </si>
   <si>
-    <t>AutoTestUser</t>
-  </si>
-  <si>
     <t>RecieverRole</t>
   </si>
   <si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Admin</t>
-  </si>
-  <si>
-    <t>AutoTestAdmin</t>
   </si>
   <si>
     <t>Issued for Approval</t>
@@ -199,6 +196,32 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="user_credentials"/>
+      <sheetName val="DocumentDetails"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>AutoTestAdmin</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>AutoTestUser</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -539,7 +562,7 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -558,10 +581,10 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -600,7 +623,7 @@
         <v>4</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>9</v>
@@ -614,16 +637,18 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="C2" t="str">
+        <f>[1]user_credentials!$B$3</f>
+        <v>AutoTestAdmin</v>
+      </c>
+      <c r="D2" t="str">
+        <f>[1]user_credentials!$B$4</f>
+        <v>AutoTestUser</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -635,7 +660,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N2" s="2" t="str">
         <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O2)</f>
@@ -645,21 +670,23 @@
         <v>5</v>
       </c>
       <c r="P2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="C3" t="str">
+        <f>[1]user_credentials!$B$3</f>
+        <v>AutoTestAdmin</v>
+      </c>
+      <c r="D3" t="str">
+        <f>[1]user_credentials!$B$4</f>
+        <v>AutoTestUser</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -671,7 +698,7 @@
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N3" t="str">
         <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O3)</f>
@@ -681,18 +708,19 @@
         <v>5</v>
       </c>
       <c r="P3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="C4" t="str">
+        <f>[1]user_credentials!$B$3</f>
+        <v>AutoTestAdmin</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -704,7 +732,7 @@
         <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N4" t="str">
         <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O4)</f>
@@ -714,18 +742,19 @@
         <v>5</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="C5" t="str">
+        <f>[1]user_credentials!$B$3</f>
+        <v>AutoTestAdmin</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -737,7 +766,7 @@
         <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N5" t="str">
         <f>CONCATENATE(ROW()-1," of ",COUNTA(A2:A100)," ",O5)</f>
@@ -747,7 +776,7 @@
         <v>5</v>
       </c>
       <c r="P5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected non-admin user in the data
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval-CancelAndClose.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval-CancelAndClose.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS_Sprint5\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_May\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Transmittals_Close_Cancel!$A$1:$R$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -555,7 +555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -646,10 +648,6 @@
         <f>[1]user_credentials!$B$3</f>
         <v>AutoTestAdmin</v>
       </c>
-      <c r="D2" t="str">
-        <f>[1]user_credentials!$B$4</f>
-        <v>AutoTestUser</v>
-      </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
@@ -684,10 +682,6 @@
         <f>[1]user_credentials!$B$3</f>
         <v>AutoTestAdmin</v>
       </c>
-      <c r="D3" t="str">
-        <f>[1]user_credentials!$B$4</f>
-        <v>AutoTestUser</v>
-      </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
@@ -719,8 +713,8 @@
         <v>22</v>
       </c>
       <c r="C4" t="str">
-        <f>[1]user_credentials!$B$3</f>
-        <v>AutoTestAdmin</v>
+        <f>[1]user_credentials!$B$4</f>
+        <v>AutoTestUser</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -753,8 +747,8 @@
         <v>22</v>
       </c>
       <c r="C5" t="str">
-        <f>[1]user_credentials!$B$3</f>
-        <v>AutoTestAdmin</v>
+        <f>[1]user_credentials!$B$4</f>
+        <v>AutoTestUser</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>

</xml_diff>